<commit_message>
include more questions (gender, age, password manager, etc.) git push git status
</commit_message>
<xml_diff>
--- a/forms/ds4owd_precourse_survey.xlsx
+++ b/forms/ds4owd_precourse_survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwalder/Documents/gitrepos/pre-course-survey/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B254B515-27C5-6141-B60D-019C8CA4224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2C94F2-BBA1-5345-AA76-CBEB2421A3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <author>tc={EC52FF30-1F93-454C-B4D1-296FBEFB8F09}</author>
   </authors>
   <commentList>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{228002C7-D79D-6449-BF9C-ECA8C631634A}">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{228002C7-D79D-6449-BF9C-ECA8C631634A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -39,7 +39,7 @@
     Not required?</t>
       </text>
     </comment>
-    <comment ref="C11" authorId="1" shapeId="0" xr:uid="{7853D72E-F52B-6C4C-BEB8-5A750C787E78}">
+    <comment ref="C16" authorId="1" shapeId="0" xr:uid="{7853D72E-F52B-6C4C-BEB8-5A750C787E78}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -47,7 +47,7 @@
     Not required?</t>
       </text>
     </comment>
-    <comment ref="C17" authorId="2" shapeId="0" xr:uid="{D9A1B66C-31BB-F14F-B0E8-85230951B9A0}">
+    <comment ref="C22" authorId="2" shapeId="0" xr:uid="{D9A1B66C-31BB-F14F-B0E8-85230951B9A0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
     Not required?</t>
       </text>
     </comment>
-    <comment ref="A56" authorId="3" shapeId="0" xr:uid="{9157A60D-B085-8742-948E-C529D1FAFAE4}">
+    <comment ref="A67" authorId="3" shapeId="0" xr:uid="{9157A60D-B085-8742-948E-C529D1FAFAE4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +63,7 @@
     There should be a "No" option as well</t>
       </text>
     </comment>
-    <comment ref="A59" authorId="4" shapeId="0" xr:uid="{EC52FF30-1F93-454C-B4D1-296FBEFB8F09}">
+    <comment ref="A70" authorId="4" shapeId="0" xr:uid="{EC52FF30-1F93-454C-B4D1-296FBEFB8F09}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="904">
   <si>
     <t>type</t>
   </si>
@@ -2473,9 +2473,6 @@
   </si>
   <si>
     <t>No, I am not interested</t>
-  </si>
-  <si>
-    <t>yes_only</t>
   </si>
   <si>
     <t>form_title</t>
@@ -2540,6 +2537,276 @@
   </si>
   <si>
     <t>Note that you must acknowledge the Code of Conduct and provide consent to be able to submit the form.</t>
+  </si>
+  <si>
+    <t>select_one list_gender</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>What is your gender?</t>
+  </si>
+  <si>
+    <t>gender_self_describe</t>
+  </si>
+  <si>
+    <t>Prefer to self-describe:</t>
+  </si>
+  <si>
+    <t>select_one list_age_group</t>
+  </si>
+  <si>
+    <t>age_group</t>
+  </si>
+  <si>
+    <t>What is your age group?</t>
+  </si>
+  <si>
+    <t>select_one list_accessibility</t>
+  </si>
+  <si>
+    <t>accessibility_needs</t>
+  </si>
+  <si>
+    <t>Do you have any accessibility needs we should be aware of?</t>
+  </si>
+  <si>
+    <t>accessibility_specify</t>
+  </si>
+  <si>
+    <t>Yes (please specify):</t>
+  </si>
+  <si>
+    <t>${gender} = 'self_describe'</t>
+  </si>
+  <si>
+    <t>${accessibility_needs} = 'yes'</t>
+  </si>
+  <si>
+    <t>list_gender</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>non_binary</t>
+  </si>
+  <si>
+    <t>Non-binary</t>
+  </si>
+  <si>
+    <t>self_describe</t>
+  </si>
+  <si>
+    <t>prefer_not_to_say_gender</t>
+  </si>
+  <si>
+    <t>Prefer not to say</t>
+  </si>
+  <si>
+    <t>list_age_group</t>
+  </si>
+  <si>
+    <t>under_18</t>
+  </si>
+  <si>
+    <t>Under 18</t>
+  </si>
+  <si>
+    <t>18_24</t>
+  </si>
+  <si>
+    <t>18–24</t>
+  </si>
+  <si>
+    <t>25_34</t>
+  </si>
+  <si>
+    <t>25–34</t>
+  </si>
+  <si>
+    <t>35_44</t>
+  </si>
+  <si>
+    <t>35–44</t>
+  </si>
+  <si>
+    <t>45_54</t>
+  </si>
+  <si>
+    <t>45–54</t>
+  </si>
+  <si>
+    <t>55_64</t>
+  </si>
+  <si>
+    <t>55–64</t>
+  </si>
+  <si>
+    <t>65_or_older</t>
+  </si>
+  <si>
+    <t>65 or older</t>
+  </si>
+  <si>
+    <t>prefer_not_to_say_age</t>
+  </si>
+  <si>
+    <t>list_accessibility</t>
+  </si>
+  <si>
+    <t>prefer_not_to_say_accessibility</t>
+  </si>
+  <si>
+    <t>list_password_storage</t>
+  </si>
+  <si>
+    <t>I don’t store them anywhere</t>
+  </si>
+  <si>
+    <t>unprotected_digital</t>
+  </si>
+  <si>
+    <t>I store them in an unprotected digital file or app (e.g., Word, Excel, email, WhatsApp)</t>
+  </si>
+  <si>
+    <t>I write them down on paper</t>
+  </si>
+  <si>
+    <t>password_manager</t>
+  </si>
+  <si>
+    <t>I use a password manager</t>
+  </si>
+  <si>
+    <t>list_web_browser</t>
+  </si>
+  <si>
+    <t>google_chrome</t>
+  </si>
+  <si>
+    <t>Google Chrome</t>
+  </si>
+  <si>
+    <t>apple_safari</t>
+  </si>
+  <si>
+    <t>Apple Safari</t>
+  </si>
+  <si>
+    <t>microsoft_edge</t>
+  </si>
+  <si>
+    <t>Microsoft Edge</t>
+  </si>
+  <si>
+    <t>mozilla_firefox</t>
+  </si>
+  <si>
+    <t>Mozilla Firefox</t>
+  </si>
+  <si>
+    <t>samsung_internet</t>
+  </si>
+  <si>
+    <t>Samsung Internet</t>
+  </si>
+  <si>
+    <t>opera</t>
+  </si>
+  <si>
+    <t>Opera</t>
+  </si>
+  <si>
+    <t>brave</t>
+  </si>
+  <si>
+    <t>Brave</t>
+  </si>
+  <si>
+    <t>vivaldi</t>
+  </si>
+  <si>
+    <t>Vivaldi</t>
+  </si>
+  <si>
+    <t>arc</t>
+  </si>
+  <si>
+    <t>Arc</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>select_one list_password_storage</t>
+  </si>
+  <si>
+    <t>password_storage</t>
+  </si>
+  <si>
+    <t>How do you usually store your passwords or credentials?</t>
+  </si>
+  <si>
+    <t>select_one list_web_browser</t>
+  </si>
+  <si>
+    <t>web_browser</t>
+  </si>
+  <si>
+    <t>Which web browser do you use most often?</t>
+  </si>
+  <si>
+    <t>web_browser_other</t>
+  </si>
+  <si>
+    <t>Other (please specify):</t>
+  </si>
+  <si>
+    <t>${web_browser} = 'other'</t>
+  </si>
+  <si>
+    <t>use_bookmarks</t>
+  </si>
+  <si>
+    <t>Do you use browser bookmarks?</t>
+  </si>
+  <si>
+    <t>use_note_taking_tool</t>
+  </si>
+  <si>
+    <t>Do you use a note-taking tool?</t>
+  </si>
+  <si>
+    <t>note_taking_tool_specify</t>
+  </si>
+  <si>
+    <t>${use_note_taking_tool} = 'yes'</t>
+  </si>
+  <si>
+    <t>Which tool to you use?</t>
+  </si>
+  <si>
+    <t>You have to answer this question with "yes" to be able to submit the form.</t>
+  </si>
+  <si>
+    <t>This question is optional.</t>
+  </si>
+  <si>
+    <t>Prefer to self-describe</t>
+  </si>
+  <si>
+    <t>Select the option that best describes your usual practice.</t>
   </si>
 </sst>
 </file>
@@ -2567,8 +2834,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2628,7 +2895,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2651,6 +2918,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2959,19 +3227,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D9" dT="2025-07-02T16:16:20.02" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{228002C7-D79D-6449-BF9C-ECA8C631634A}">
+  <threadedComment ref="D14" dT="2025-07-02T16:16:20.02" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{228002C7-D79D-6449-BF9C-ECA8C631634A}">
     <text>Not required?</text>
   </threadedComment>
-  <threadedComment ref="C11" dT="2025-07-02T16:16:38.78" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{7853D72E-F52B-6C4C-BEB8-5A750C787E78}">
+  <threadedComment ref="C16" dT="2025-07-02T16:16:38.78" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{7853D72E-F52B-6C4C-BEB8-5A750C787E78}">
     <text>Not required?</text>
   </threadedComment>
-  <threadedComment ref="C17" dT="2025-07-02T16:16:45.94" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{D9A1B66C-31BB-F14F-B0E8-85230951B9A0}">
+  <threadedComment ref="C22" dT="2025-07-02T16:16:45.94" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{D9A1B66C-31BB-F14F-B0E8-85230951B9A0}">
     <text>Not required?</text>
   </threadedComment>
-  <threadedComment ref="A56" dT="2025-07-02T16:15:50.10" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{9157A60D-B085-8742-948E-C529D1FAFAE4}">
+  <threadedComment ref="A67" dT="2025-07-02T16:15:50.10" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{9157A60D-B085-8742-948E-C529D1FAFAE4}">
     <text>There should be a "No" option as well</text>
   </threadedComment>
-  <threadedComment ref="A59" dT="2025-07-03T09:11:31.61" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{EC52FF30-1F93-454C-B4D1-296FBEFB8F09}">
+  <threadedComment ref="A70" dT="2025-07-03T09:11:31.61" personId="{5C321BBF-5658-5540-AD42-8E179DB5663B}" id="{EC52FF30-1F93-454C-B4D1-296FBEFB8F09}">
     <text>Added this question that is only displayed if code_conduct and data_privacy are answered with "Yes". This means that the form can only be submitted if both are accepted.</text>
   </threadedComment>
 </ThreadedComments>
@@ -2979,11 +3247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3035,10 +3303,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>806</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>807</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3144,473 +3412,491 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>814</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>815</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>816</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="J9" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>36</v>
+      <c r="F9" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>817</v>
+      </c>
+      <c r="C10" t="s">
+        <v>818</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>819</v>
+      </c>
+      <c r="B11" t="s">
+        <v>820</v>
+      </c>
+      <c r="C11" t="s">
+        <v>821</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>901</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>822</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>823</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>824</v>
       </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
+      <c r="F12" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>825</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>826</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
+      <c r="G13" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="G14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>45</v>
+      <c r="F14" t="s">
+        <v>901</v>
+      </c>
+      <c r="J14" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>90</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
-      </c>
-      <c r="D44" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3618,13 +3904,13 @@
         <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3632,13 +3918,13 @@
         <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3646,109 +3932,142 @@
         <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>123</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>809</v>
+        <v>105</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>884</v>
+      </c>
+      <c r="B53" t="s">
+        <v>885</v>
+      </c>
+      <c r="C53" t="s">
+        <v>886</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" t="s">
+        <v>903</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>887</v>
       </c>
       <c r="B54" t="s">
-        <v>813</v>
+        <v>888</v>
       </c>
       <c r="C54" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>132</v>
+        <v>889</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>890</v>
+      </c>
+      <c r="C55" t="s">
+        <v>891</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>893</v>
       </c>
       <c r="C56" t="s">
-        <v>134</v>
+        <v>894</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
@@ -3756,35 +4075,174 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>895</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>896</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>897</v>
+      </c>
+      <c r="C58" t="s">
+        <v>899</v>
+      </c>
+      <c r="D58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>808</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" t="s">
+        <v>812</v>
+      </c>
+      <c r="C65" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>808</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>808</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>808</v>
+      </c>
+      <c r="B70" t="s">
         <v>809</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C70" t="s">
         <v>810</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D70" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" t="s">
         <v>811</v>
-      </c>
-      <c r="G59" t="s">
-        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -3795,10 +4253,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C334"/>
+  <dimension ref="A1:C363"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A331" sqref="A331"/>
+    <sheetView topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="I340" sqref="I340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7418,7 +7876,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B329" s="5" t="s">
         <v>17</v>
@@ -7429,7 +7887,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B330" s="5" t="s">
         <v>33</v>
@@ -7472,14 +7930,333 @@
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A334" s="5" t="s">
-        <v>799</v>
-      </c>
-      <c r="B334" s="5" t="s">
+      <c r="A334" s="12" t="s">
+        <v>829</v>
+      </c>
+      <c r="B334" s="12" t="s">
+        <v>830</v>
+      </c>
+      <c r="C334" s="12" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A335" s="12" t="s">
+        <v>829</v>
+      </c>
+      <c r="B335" s="12" t="s">
+        <v>832</v>
+      </c>
+      <c r="C335" s="12" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A336" s="12" t="s">
+        <v>829</v>
+      </c>
+      <c r="B336" s="12" t="s">
+        <v>834</v>
+      </c>
+      <c r="C336" s="12" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A337" s="12" t="s">
+        <v>829</v>
+      </c>
+      <c r="B337" s="12" t="s">
+        <v>836</v>
+      </c>
+      <c r="C337" s="12" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A338" s="12" t="s">
+        <v>829</v>
+      </c>
+      <c r="B338" s="12" t="s">
+        <v>837</v>
+      </c>
+      <c r="C338" s="12" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A339" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B339" s="12" t="s">
+        <v>840</v>
+      </c>
+      <c r="C339" s="12" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A340" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B340" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="C340" s="12" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A341" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B341" s="12" t="s">
+        <v>844</v>
+      </c>
+      <c r="C341" s="12" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A342" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B342" s="12" t="s">
+        <v>846</v>
+      </c>
+      <c r="C342" s="12" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B343" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="C343" s="12" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B344" s="12" t="s">
+        <v>850</v>
+      </c>
+      <c r="C344" s="12" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A345" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B345" s="12" t="s">
+        <v>852</v>
+      </c>
+      <c r="C345" s="12" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A346" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="B346" s="12" t="s">
+        <v>854</v>
+      </c>
+      <c r="C346" s="12" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A347" s="12" t="s">
+        <v>855</v>
+      </c>
+      <c r="B347" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C334" s="5" t="s">
+      <c r="C347" s="12" t="s">
         <v>790</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A348" s="12" t="s">
+        <v>855</v>
+      </c>
+      <c r="B348" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C348" s="12" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A349" s="12" t="s">
+        <v>855</v>
+      </c>
+      <c r="B349" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C349" s="12" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A350" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="B350" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C350" s="12" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A351" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="B351" s="12" t="s">
+        <v>859</v>
+      </c>
+      <c r="C351" s="12" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A352" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="B352" s="12" t="s">
+        <v>662</v>
+      </c>
+      <c r="C352" s="12" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A353" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="B353" s="12" t="s">
+        <v>862</v>
+      </c>
+      <c r="C353" s="12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A354" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B354" s="12" t="s">
+        <v>865</v>
+      </c>
+      <c r="C354" s="12" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A355" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B355" s="12" t="s">
+        <v>867</v>
+      </c>
+      <c r="C355" s="12" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A356" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B356" s="12" t="s">
+        <v>869</v>
+      </c>
+      <c r="C356" s="12" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A357" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B357" s="12" t="s">
+        <v>871</v>
+      </c>
+      <c r="C357" s="12" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A358" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B358" s="12" t="s">
+        <v>873</v>
+      </c>
+      <c r="C358" s="12" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A359" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B359" s="12" t="s">
+        <v>875</v>
+      </c>
+      <c r="C359" s="12" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A360" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B360" s="12" t="s">
+        <v>877</v>
+      </c>
+      <c r="C360" s="12" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A361" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B361" s="12" t="s">
+        <v>879</v>
+      </c>
+      <c r="C361" s="12" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A362" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B362" s="12" t="s">
+        <v>881</v>
+      </c>
+      <c r="C362" s="12" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A363" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B363" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C363" s="12" t="s">
+        <v>883</v>
       </c>
     </row>
   </sheetData>
@@ -7504,21 +8281,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>800</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>801</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>803</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>804</v>
       </c>
       <c r="C2" s="5">
         <v>20250701</v>

</xml_diff>